<commit_message>
add some more changes
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artem/PyProjects/PercentageCalculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111F7E8F-BD84-3043-9308-E6149E8BDB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81338835-9131-104A-943C-7AF6C09D0582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="900" windowWidth="29100" windowHeight="17180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>№ п/п</t>
   </si>
@@ -53,13 +53,25 @@
     <t>Сумма коммерческого займа</t>
   </si>
   <si>
+    <t>21.10.2024</t>
+  </si>
+  <si>
+    <t>25.10.2024</t>
+  </si>
+  <si>
+    <t>18.10.2024</t>
+  </si>
+  <si>
     <t>30.10.2024</t>
   </si>
   <si>
-    <t>18.10.2024</t>
+    <t>31.10.2024</t>
   </si>
   <si>
     <t>15.10.2024</t>
+  </si>
+  <si>
+    <t>29.10.2024</t>
   </si>
 </sst>
 </file>
@@ -597,13 +609,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
@@ -680,22 +695,22 @@
         <v>12066.8</v>
       </c>
       <c r="E3">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3">
-        <v>6066.7999999999993</v>
+        <v>2066.7999999999988</v>
       </c>
       <c r="H3">
         <v>3.3055000000000001E-2</v>
       </c>
       <c r="I3">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="J3">
-        <v>60.16</v>
+        <v>14.35</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -703,33 +718,36 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2766291</v>
+        <v>2766285</v>
       </c>
       <c r="C4" s="2">
-        <v>45492</v>
+        <v>45485</v>
       </c>
       <c r="D4">
-        <v>6666.12</v>
+        <v>12066.8</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>12500</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
       <c r="G4">
-        <v>6666.12</v>
+        <v>-433.20000000000073</v>
       </c>
       <c r="H4">
         <v>3.3055000000000001E-2</v>
       </c>
       <c r="I4">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="J4">
-        <v>68.31</v>
+        <v>-0.56999999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2766291</v>
@@ -741,27 +759,24 @@
         <v>6666.12</v>
       </c>
       <c r="E5">
-        <v>2000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>4666.12</v>
+        <v>6666.12</v>
       </c>
       <c r="H5">
         <v>3.3055000000000001E-2</v>
       </c>
       <c r="I5">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="J5">
-        <v>27.76</v>
+        <v>68.31</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2766291</v>
@@ -773,54 +788,150 @@
         <v>6666.12</v>
       </c>
       <c r="E6">
-        <v>6250.8</v>
+        <v>2000</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G6">
-        <v>415.31999999999971</v>
+        <v>4666.12</v>
       </c>
       <c r="H6">
         <v>3.3055000000000001E-2</v>
       </c>
       <c r="I6">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J6">
-        <v>1.65</v>
+        <v>27.76</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2766291</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45492</v>
+      </c>
+      <c r="D7">
+        <v>6666.12</v>
+      </c>
+      <c r="E7">
+        <v>6250.8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>415.31999999999971</v>
+      </c>
+      <c r="H7">
+        <v>3.3055000000000001E-2</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2766291</v>
+      </c>
+      <c r="C8" s="2">
+        <v>45492</v>
+      </c>
+      <c r="D8">
+        <v>6666.12</v>
+      </c>
+      <c r="E8">
+        <v>6665.8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>0.31999999999970902</v>
+      </c>
+      <c r="H8">
+        <v>3.3055000000000001E-2</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2766294</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45527</v>
+      </c>
+      <c r="D9">
+        <v>11155.81</v>
+      </c>
+      <c r="E9">
+        <v>11005</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>150.80999999999949</v>
+      </c>
+      <c r="H9">
+        <v>3.3055000000000001E-2</v>
+      </c>
+      <c r="I9">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="J9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
         <v>2766294</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C10" s="2">
         <v>45527</v>
       </c>
-      <c r="D7">
+      <c r="D10">
         <v>11155.81</v>
       </c>
-      <c r="E7">
-        <v>11005</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7">
-        <v>150.80999999999949</v>
-      </c>
-      <c r="H7">
-        <v>3.3055000000000001E-2</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <v>0.25</v>
+      <c r="E10">
+        <v>11008.15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>147.65999999999991</v>
+      </c>
+      <c r="H10">
+        <v>3.3055000000000001E-2</v>
+      </c>
+      <c r="I10">
+        <v>14</v>
+      </c>
+      <c r="J10">
+        <v>0.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>